<commit_message>
Actualizacion hasta el ejercicio 3.11
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E92DA6-E386-4E47-8681-CA7BA162111E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389ACE91-50BE-4D80-A0B4-B7591B53EF9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejercicio 2.83" sheetId="1" r:id="rId1"/>
-    <sheet name="Ejercicios 3.1-" sheetId="2" r:id="rId2"/>
+    <sheet name="Ejercicios 3.1-3.11" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -137,6 +137,27 @@
   <si>
     <t>Demanda de un bien X</t>
   </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>dP</t>
+  </si>
+  <si>
+    <t>c+dP</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +167,7 @@
     <numFmt numFmtId="164" formatCode="yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -267,7 +288,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -354,12 +375,13 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
@@ -1125,6 +1147,1554 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500"/>
+              <a:t>Demanda</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500" baseline="0"/>
+              <a:t> de un bien X.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1500"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejercicios 3.1-3.11'!$A$99</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Demanda de un bien X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ejercicios 3.1-3.11'!$F$145:$F$149</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ejercicios 3.1-3.11'!$A$145:$A$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-73E8-4AC5-BCF0-8ADB66942429}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> del bien X</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500"/>
+              <a:t>Oferta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500" baseline="0"/>
+              <a:t> de un bien X.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1500"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejercicios 3.1-3.11'!$A$99</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Demanda de un bien X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ejercicios 3.1-3.11'!$F$161:$F$165</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ejercicios 3.1-3.11'!$A$161:$A$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B97-49E2-860E-4968F10309EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> del bien X</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500"/>
+              <a:t>Oferta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500" baseline="0"/>
+              <a:t> de un bien X.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1500"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ejercicios 3.1-3.11'!$A$99</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Demanda de un bien X</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ejercicios 3.1-3.11'!$F$178:$F$182</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ejercicios 3.1-3.11'!$A$178:$A$182</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E15A-4520-9885-55F3CFCE62FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> del bien X</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -1220,7 +2790,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$B$2</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1254,7 +2824,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$3:$A$8</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1281,7 +2851,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$B$3:$B$8</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1318,7 +2888,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$B$2</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1365,7 +2935,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$3:$A$8</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1392,7 +2962,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$B$3:$B$8</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1840,7 +3410,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$B$18</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1874,7 +3444,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$19:$A$23</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$19:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1898,7 +3468,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$B$19:$B$23</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$19:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1932,7 +3502,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$B$18</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1979,7 +3549,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$19:$A$24</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$19:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2003,7 +3573,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$B$19:$B$24</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$19:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2448,7 +4018,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$B$35</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2495,7 +4065,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$36:$A$41</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$36:$A$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2522,7 +4092,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$B$36:$B$41</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$36:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2971,7 +4541,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$B$35</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3018,7 +4588,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$53:$A$57</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$53:$A$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3042,7 +4612,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$B$53:$B$57</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$B$53:$B$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3488,7 +5058,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$E$68</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$E$68</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3535,7 +5105,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$D$69:$D$77</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$D$69:$D$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -3571,7 +5141,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$E$69:$E$77</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$E$69:$E$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -4029,7 +5599,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$A$99</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$99</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4076,7 +5646,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$F$94:$F$98</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$F$94:$F$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4100,7 +5670,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$94:$A$98</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$94:$A$98</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4545,7 +6115,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$A$99</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$99</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4592,7 +6162,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$F$112:$F$116</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$F$112:$F$116</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4616,7 +6186,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$112:$A$116</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$112:$A$116</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5061,7 +6631,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ejercicios 3.1-'!$A$99</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$99</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5108,7 +6678,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$F$129:$F$133</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$F$129:$F$133</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5132,7 +6702,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Ejercicios 3.1-'!$A$129:$A$133</c:f>
+              <c:f>'Ejercicios 3.1-3.11'!$A$129:$A$133</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5522,6 +7092,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6353,6 +8043,1659 @@
       <a:ln>
         <a:noFill/>
       </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -11111,6 +14454,120 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Gráfico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{074485ED-2A05-43F1-BDF6-B6EE77FF4686}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Gráfico 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B5226F-B21F-4DAC-BD05-4B6670967553}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Gráfico 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78342177-AA7E-439D-A29B-1606D5943072}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12337,10 +15794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4827C6-795B-4E7E-9616-5B8D2BEECDBA}">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="H127" sqref="H127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D187" sqref="D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12349,10 +15806,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="38">
+      <c r="A1" s="41">
         <v>3.1</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
@@ -12411,10 +15868,10 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="38">
+      <c r="A17" s="41">
         <v>3.2</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="41"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
@@ -12465,10 +15922,10 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="38">
+      <c r="A34" s="41">
         <v>3.3</v>
       </c>
-      <c r="B34" s="38"/>
+      <c r="B34" s="41"/>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
@@ -12527,10 +15984,10 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="38">
+      <c r="A51" s="41">
         <v>3.4</v>
       </c>
-      <c r="B51" s="38"/>
+      <c r="B51" s="41"/>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
@@ -12581,14 +16038,14 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="38">
+      <c r="A67" s="41">
         <v>3.5</v>
       </c>
-      <c r="B67" s="38"/>
-      <c r="D67" s="38">
+      <c r="B67" s="41"/>
+      <c r="D67" s="41">
         <v>3.5</v>
       </c>
-      <c r="E67" s="38"/>
+      <c r="E67" s="41"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
@@ -12615,7 +16072,7 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <f>SUMIF($A$69:$A$90,D69,$B$69:$B$90)</f>
+        <f t="shared" ref="E69:E77" si="0">SUMIF($A$69:$A$90,D69,$B$69:$B$90)</f>
         <v>120</v>
       </c>
     </row>
@@ -12630,7 +16087,7 @@
         <v>5</v>
       </c>
       <c r="E70">
-        <f>SUMIF($A$69:$A$90,D70,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
@@ -12645,7 +16102,7 @@
         <v>10</v>
       </c>
       <c r="E71">
-        <f>SUMIF($A$69:$A$90,D71,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
@@ -12660,7 +16117,7 @@
         <v>15</v>
       </c>
       <c r="E72">
-        <f>SUMIF($A$69:$A$90,D72,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
@@ -12675,7 +16132,7 @@
         <v>20</v>
       </c>
       <c r="E73">
-        <f>SUMIF($A$69:$A$90,D73,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>67</v>
       </c>
     </row>
@@ -12690,7 +16147,7 @@
         <v>25</v>
       </c>
       <c r="E74">
-        <f>SUMIF($A$69:$A$90,D74,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
@@ -12705,7 +16162,7 @@
         <v>30</v>
       </c>
       <c r="E75">
-        <f>SUMIF($A$69:$A$90,D75,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
@@ -12720,7 +16177,7 @@
         <v>35</v>
       </c>
       <c r="E76">
-        <f>SUMIF($A$69:$A$90,D76,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
@@ -12735,7 +16192,7 @@
         <v>40</v>
       </c>
       <c r="E77">
-        <f>SUMIF($A$69:$A$90,D77,$B$69:$B$90)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -12844,14 +16301,14 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="38">
+      <c r="A92" s="41">
         <v>3.6</v>
       </c>
-      <c r="B92" s="38"/>
-      <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="38"/>
+      <c r="B92" s="41"/>
+      <c r="C92" s="41"/>
+      <c r="D92" s="41"/>
+      <c r="E92" s="41"/>
+      <c r="F92" s="41"/>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
@@ -12880,7 +16337,7 @@
       <c r="B94">
         <v>60</v>
       </c>
-      <c r="C94" s="39">
+      <c r="C94" s="38">
         <v>0.5</v>
       </c>
       <c r="D94">
@@ -12903,19 +16360,19 @@
       <c r="B95">
         <v>60</v>
       </c>
-      <c r="C95" s="39">
+      <c r="C95" s="38">
         <v>0.5</v>
       </c>
       <c r="D95">
-        <f t="shared" ref="D95:D98" si="0">C95*A95</f>
+        <f t="shared" ref="D95:D98" si="1">C95*A95</f>
         <v>40</v>
       </c>
       <c r="E95">
-        <f t="shared" ref="E95:E98" si="1">B95-D95</f>
+        <f t="shared" ref="E95:E98" si="2">B95-D95</f>
         <v>20</v>
       </c>
       <c r="F95">
-        <f t="shared" ref="F95:F98" si="2">E95</f>
+        <f t="shared" ref="F95:F98" si="3">E95</f>
         <v>20</v>
       </c>
     </row>
@@ -12926,19 +16383,19 @@
       <c r="B96">
         <v>60</v>
       </c>
-      <c r="C96" s="39">
+      <c r="C96" s="38">
         <v>0.5</v>
       </c>
       <c r="D96">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="E96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="F96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
@@ -12949,19 +16406,19 @@
       <c r="B97">
         <v>60</v>
       </c>
-      <c r="C97" s="39">
+      <c r="C97" s="38">
         <v>0.5</v>
       </c>
       <c r="D97">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="E97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="F97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
@@ -12972,19 +16429,19 @@
       <c r="B98">
         <v>60</v>
       </c>
-      <c r="C98" s="39">
+      <c r="C98" s="38">
         <v>0.5</v>
       </c>
       <c r="D98">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="E98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -12994,14 +16451,14 @@
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="38">
+      <c r="A110" s="41">
         <v>3.7</v>
       </c>
-      <c r="B110" s="38"/>
-      <c r="C110" s="38"/>
-      <c r="D110" s="38"/>
-      <c r="E110" s="38"/>
-      <c r="F110" s="38"/>
+      <c r="B110" s="41"/>
+      <c r="C110" s="41"/>
+      <c r="D110" s="41"/>
+      <c r="E110" s="41"/>
+      <c r="F110" s="41"/>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
@@ -13030,19 +16487,19 @@
       <c r="B112">
         <v>45</v>
       </c>
-      <c r="C112" s="40">
+      <c r="C112" s="39">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D112" s="41">
+      <c r="D112" s="40">
         <f>C112*A112</f>
         <v>20</v>
       </c>
-      <c r="E112" s="41">
+      <c r="E112" s="40">
         <f>B112-D112</f>
         <v>25</v>
       </c>
-      <c r="F112" s="41">
+      <c r="F112" s="40">
         <f>E112</f>
         <v>25</v>
       </c>
@@ -13054,20 +16511,20 @@
       <c r="B113">
         <v>45</v>
       </c>
-      <c r="C113" s="40">
-        <f t="shared" ref="C113:C116" si="3">1/3</f>
+      <c r="C113" s="39">
+        <f t="shared" ref="C113:C116" si="4">1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D113" s="41">
-        <f t="shared" ref="D113:D116" si="4">C113*A113</f>
+      <c r="D113" s="40">
+        <f t="shared" ref="D113:D116" si="5">C113*A113</f>
         <v>26.666666666666664</v>
       </c>
-      <c r="E113" s="41">
-        <f t="shared" ref="E113:E116" si="5">B113-D113</f>
+      <c r="E113" s="40">
+        <f t="shared" ref="E113:E116" si="6">B113-D113</f>
         <v>18.333333333333336</v>
       </c>
-      <c r="F113" s="41">
-        <f t="shared" ref="F113:F116" si="6">E113</f>
+      <c r="F113" s="40">
+        <f t="shared" ref="F113:F116" si="7">E113</f>
         <v>18.333333333333336</v>
       </c>
     </row>
@@ -13078,20 +16535,20 @@
       <c r="B114">
         <v>45</v>
       </c>
-      <c r="C114" s="40">
-        <f t="shared" si="3"/>
+      <c r="C114" s="39">
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D114" s="41">
-        <f t="shared" si="4"/>
+      <c r="D114" s="40">
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="E114" s="41">
+      <c r="E114" s="40">
         <f>B114-D114</f>
         <v>15</v>
       </c>
-      <c r="F114" s="41">
-        <f t="shared" si="6"/>
+      <c r="F114" s="40">
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
     </row>
@@ -13102,20 +16559,20 @@
       <c r="B115">
         <v>45</v>
       </c>
-      <c r="C115" s="40">
-        <f t="shared" si="3"/>
+      <c r="C115" s="39">
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D115" s="41">
+      <c r="D115" s="40">
         <f>C115*A115</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E115" s="41">
-        <f t="shared" si="5"/>
+      <c r="E115" s="40">
+        <f t="shared" si="6"/>
         <v>11.666666666666671</v>
       </c>
-      <c r="F115" s="41">
-        <f t="shared" si="6"/>
+      <c r="F115" s="40">
+        <f t="shared" si="7"/>
         <v>11.666666666666671</v>
       </c>
     </row>
@@ -13126,32 +16583,32 @@
       <c r="B116">
         <v>45</v>
       </c>
-      <c r="C116" s="40">
-        <f t="shared" si="3"/>
+      <c r="C116" s="39">
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D116" s="41">
-        <f t="shared" si="4"/>
+      <c r="D116" s="40">
+        <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="E116" s="41">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="F116" s="41">
+      <c r="E116" s="40">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
+      <c r="F116" s="40">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="38">
+      <c r="A127" s="41">
         <v>3.8</v>
       </c>
-      <c r="B127" s="38"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38"/>
-      <c r="F127" s="38"/>
+      <c r="B127" s="41"/>
+      <c r="C127" s="41"/>
+      <c r="D127" s="41"/>
+      <c r="E127" s="41"/>
+      <c r="F127" s="41"/>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
@@ -13180,18 +16637,18 @@
       <c r="B129">
         <v>80</v>
       </c>
-      <c r="C129" s="40">
+      <c r="C129" s="39">
         <v>0.1</v>
       </c>
-      <c r="D129" s="41">
+      <c r="D129" s="40">
         <f>C129*A129</f>
         <v>0</v>
       </c>
-      <c r="E129" s="41">
+      <c r="E129" s="40">
         <f>B129-D129</f>
         <v>80</v>
       </c>
-      <c r="F129" s="41">
+      <c r="F129" s="40">
         <f>E129</f>
         <v>80</v>
       </c>
@@ -13203,19 +16660,19 @@
       <c r="B130">
         <v>80</v>
       </c>
-      <c r="C130" s="40">
+      <c r="C130" s="39">
         <v>0.1</v>
       </c>
-      <c r="D130" s="41">
-        <f t="shared" ref="D130:D131" si="7">C130*A130</f>
+      <c r="D130" s="40">
+        <f t="shared" ref="D130:D131" si="8">C130*A130</f>
         <v>1</v>
       </c>
-      <c r="E130" s="41">
-        <f t="shared" ref="E130" si="8">B130-D130</f>
+      <c r="E130" s="40">
+        <f t="shared" ref="E130" si="9">B130-D130</f>
         <v>79</v>
       </c>
-      <c r="F130" s="41">
-        <f t="shared" ref="F130:F133" si="9">E130</f>
+      <c r="F130" s="40">
+        <f t="shared" ref="F130:F133" si="10">E130</f>
         <v>79</v>
       </c>
     </row>
@@ -13226,19 +16683,19 @@
       <c r="B131">
         <v>80</v>
       </c>
-      <c r="C131" s="40">
+      <c r="C131" s="39">
         <v>0.1</v>
       </c>
-      <c r="D131" s="41">
-        <f t="shared" si="7"/>
+      <c r="D131" s="40">
+        <f t="shared" si="8"/>
         <v>2.5</v>
       </c>
-      <c r="E131" s="41">
+      <c r="E131" s="40">
         <f>B131-D131</f>
         <v>77.5</v>
       </c>
-      <c r="F131" s="41">
-        <f t="shared" si="9"/>
+      <c r="F131" s="40">
+        <f t="shared" si="10"/>
         <v>77.5</v>
       </c>
     </row>
@@ -13249,19 +16706,19 @@
       <c r="B132">
         <v>80</v>
       </c>
-      <c r="C132" s="40">
+      <c r="C132" s="39">
         <v>0.1</v>
       </c>
-      <c r="D132" s="41">
+      <c r="D132" s="40">
         <f>C132*A132</f>
         <v>8</v>
       </c>
-      <c r="E132" s="41">
-        <f t="shared" ref="E132:E133" si="10">B132-D132</f>
+      <c r="E132" s="40">
+        <f t="shared" ref="E132:E133" si="11">B132-D132</f>
         <v>72</v>
       </c>
-      <c r="F132" s="41">
-        <f t="shared" si="9"/>
+      <c r="F132" s="40">
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
     </row>
@@ -13272,27 +16729,470 @@
       <c r="B133">
         <v>80</v>
       </c>
-      <c r="C133" s="40">
+      <c r="C133" s="39">
         <v>0.1</v>
       </c>
-      <c r="D133" s="41">
-        <f t="shared" ref="D133" si="11">C133*A133</f>
+      <c r="D133" s="40">
+        <f t="shared" ref="D133" si="12">C133*A133</f>
         <v>15</v>
       </c>
-      <c r="E133" s="41">
+      <c r="E133" s="40">
+        <f t="shared" si="11"/>
+        <v>65</v>
+      </c>
+      <c r="F133" s="40">
         <f t="shared" si="10"/>
         <v>65</v>
       </c>
-      <c r="F133" s="41">
-        <f t="shared" si="9"/>
-        <v>65</v>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B143" s="41"/>
+      <c r="C143" s="41"/>
+      <c r="D143" s="41"/>
+      <c r="E143" s="41"/>
+      <c r="F143" s="41"/>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" t="s">
+        <v>28</v>
+      </c>
+      <c r="B144" t="s">
+        <v>29</v>
+      </c>
+      <c r="C144" t="s">
+        <v>30</v>
+      </c>
+      <c r="D144" t="s">
+        <v>31</v>
+      </c>
+      <c r="E144" t="s">
+        <v>32</v>
+      </c>
+      <c r="F144" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145">
+        <v>50</v>
+      </c>
+      <c r="B145">
+        <v>220</v>
+      </c>
+      <c r="C145" s="42">
+        <v>4</v>
+      </c>
+      <c r="D145" s="40">
+        <f>C145*A145</f>
+        <v>200</v>
+      </c>
+      <c r="E145" s="40">
+        <f>B145-D145</f>
+        <v>20</v>
+      </c>
+      <c r="F145" s="40">
+        <f>E145</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146">
+        <v>40</v>
+      </c>
+      <c r="B146">
+        <v>220</v>
+      </c>
+      <c r="C146" s="42">
+        <v>4</v>
+      </c>
+      <c r="D146" s="40">
+        <f t="shared" ref="D146:D147" si="13">C146*A146</f>
+        <v>160</v>
+      </c>
+      <c r="E146" s="40">
+        <f t="shared" ref="E146" si="14">B146-D146</f>
+        <v>60</v>
+      </c>
+      <c r="F146" s="40">
+        <f t="shared" ref="F146:F149" si="15">E146</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147">
+        <v>30</v>
+      </c>
+      <c r="B147">
+        <v>220</v>
+      </c>
+      <c r="C147" s="42">
+        <v>4</v>
+      </c>
+      <c r="D147" s="40">
+        <f t="shared" si="13"/>
+        <v>120</v>
+      </c>
+      <c r="E147" s="40">
+        <f>B147-D147</f>
+        <v>100</v>
+      </c>
+      <c r="F147" s="40">
+        <f t="shared" si="15"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148">
+        <v>20</v>
+      </c>
+      <c r="B148">
+        <v>220</v>
+      </c>
+      <c r="C148" s="42">
+        <v>4</v>
+      </c>
+      <c r="D148" s="40">
+        <f>C148*A148</f>
+        <v>80</v>
+      </c>
+      <c r="E148" s="40">
+        <f t="shared" ref="E148:E149" si="16">B148-D148</f>
+        <v>140</v>
+      </c>
+      <c r="F148" s="40">
+        <f t="shared" si="15"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149">
+        <v>10</v>
+      </c>
+      <c r="B149">
+        <v>220</v>
+      </c>
+      <c r="C149" s="42">
+        <v>4</v>
+      </c>
+      <c r="D149" s="40">
+        <f t="shared" ref="D149" si="17">C149*A149</f>
+        <v>40</v>
+      </c>
+      <c r="E149" s="40">
+        <f t="shared" si="16"/>
+        <v>180</v>
+      </c>
+      <c r="F149" s="40">
+        <f t="shared" si="15"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B159" s="41"/>
+      <c r="C159" s="41"/>
+      <c r="D159" s="41"/>
+      <c r="E159" s="41"/>
+      <c r="F159" s="41"/>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" t="s">
+        <v>28</v>
+      </c>
+      <c r="B160" t="s">
+        <v>37</v>
+      </c>
+      <c r="C160" t="s">
+        <v>38</v>
+      </c>
+      <c r="D160" t="s">
+        <v>39</v>
+      </c>
+      <c r="E160" t="s">
+        <v>40</v>
+      </c>
+      <c r="F160" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>20</v>
+      </c>
+      <c r="C161" s="39">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="D161" s="40">
+        <f>C161*A161</f>
+        <v>0.5</v>
+      </c>
+      <c r="E161" s="40">
+        <f>B161+D161</f>
+        <v>20.5</v>
+      </c>
+      <c r="F161" s="40">
+        <f>E161</f>
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162">
+        <v>2</v>
+      </c>
+      <c r="B162">
+        <v>20</v>
+      </c>
+      <c r="C162" s="39">
+        <f t="shared" ref="C162:C165" si="18">1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="D162" s="40">
+        <f t="shared" ref="D162:D163" si="19">C162*A162</f>
+        <v>1</v>
+      </c>
+      <c r="E162" s="40">
+        <f t="shared" ref="E162:E165" si="20">B162+D162</f>
+        <v>21</v>
+      </c>
+      <c r="F162" s="40">
+        <f t="shared" ref="F162:F165" si="21">E162</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163">
+        <v>3</v>
+      </c>
+      <c r="B163">
+        <v>20</v>
+      </c>
+      <c r="C163" s="39">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="D163" s="40">
+        <f t="shared" si="19"/>
+        <v>1.5</v>
+      </c>
+      <c r="E163" s="40">
+        <f t="shared" si="20"/>
+        <v>21.5</v>
+      </c>
+      <c r="F163" s="40">
+        <f t="shared" si="21"/>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164">
+        <v>4</v>
+      </c>
+      <c r="B164">
+        <v>20</v>
+      </c>
+      <c r="C164" s="39">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="D164" s="40">
+        <f>C164*A164</f>
+        <v>2</v>
+      </c>
+      <c r="E164" s="40">
+        <f t="shared" si="20"/>
+        <v>22</v>
+      </c>
+      <c r="F164" s="40">
+        <f t="shared" si="21"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165">
+        <v>5</v>
+      </c>
+      <c r="B165">
+        <v>20</v>
+      </c>
+      <c r="C165" s="39">
+        <f t="shared" si="18"/>
+        <v>0.5</v>
+      </c>
+      <c r="D165" s="40">
+        <f t="shared" ref="D165" si="22">C165*A165</f>
+        <v>2.5</v>
+      </c>
+      <c r="E165" s="40">
+        <f t="shared" si="20"/>
+        <v>22.5</v>
+      </c>
+      <c r="F165" s="40">
+        <f t="shared" si="21"/>
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B176" s="41"/>
+      <c r="C176" s="41"/>
+      <c r="D176" s="41"/>
+      <c r="E176" s="41"/>
+      <c r="F176" s="41"/>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" t="s">
+        <v>28</v>
+      </c>
+      <c r="B177" t="s">
+        <v>37</v>
+      </c>
+      <c r="C177" t="s">
+        <v>38</v>
+      </c>
+      <c r="D177" t="s">
+        <v>39</v>
+      </c>
+      <c r="E177" t="s">
+        <v>40</v>
+      </c>
+      <c r="F177" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178">
+        <v>1</v>
+      </c>
+      <c r="B178">
+        <v>20</v>
+      </c>
+      <c r="C178" s="42">
+        <v>2</v>
+      </c>
+      <c r="D178" s="40">
+        <f>C178*A178</f>
+        <v>2</v>
+      </c>
+      <c r="E178" s="40">
+        <f>B178+D178</f>
+        <v>22</v>
+      </c>
+      <c r="F178" s="40">
+        <f>E178</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179">
+        <v>2</v>
+      </c>
+      <c r="B179">
+        <v>20</v>
+      </c>
+      <c r="C179" s="42">
+        <v>2</v>
+      </c>
+      <c r="D179" s="40">
+        <f t="shared" ref="D179:D180" si="23">C179*A179</f>
+        <v>4</v>
+      </c>
+      <c r="E179" s="40">
+        <f t="shared" ref="E179:E182" si="24">B179+D179</f>
+        <v>24</v>
+      </c>
+      <c r="F179" s="40">
+        <f t="shared" ref="F179:F182" si="25">E179</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180">
+        <v>3</v>
+      </c>
+      <c r="B180">
+        <v>20</v>
+      </c>
+      <c r="C180" s="42">
+        <v>2</v>
+      </c>
+      <c r="D180" s="40">
+        <f t="shared" si="23"/>
+        <v>6</v>
+      </c>
+      <c r="E180" s="40">
+        <f t="shared" si="24"/>
+        <v>26</v>
+      </c>
+      <c r="F180" s="40">
+        <f t="shared" si="25"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181">
+        <v>4</v>
+      </c>
+      <c r="B181">
+        <v>20</v>
+      </c>
+      <c r="C181" s="42">
+        <v>2</v>
+      </c>
+      <c r="D181" s="40">
+        <f>C181*A181</f>
+        <v>8</v>
+      </c>
+      <c r="E181" s="40">
+        <f t="shared" si="24"/>
+        <v>28</v>
+      </c>
+      <c r="F181" s="40">
+        <f t="shared" si="25"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182">
+        <v>5</v>
+      </c>
+      <c r="B182">
+        <v>20</v>
+      </c>
+      <c r="C182" s="42">
+        <v>2</v>
+      </c>
+      <c r="D182" s="40">
+        <f t="shared" ref="D182" si="26">C182*A182</f>
+        <v>10</v>
+      </c>
+      <c r="E182" s="40">
+        <f t="shared" si="24"/>
+        <v>30</v>
+      </c>
+      <c r="F182" s="40">
+        <f t="shared" si="25"/>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="D69:D77">
     <sortCondition ref="D69:D77"/>
   </sortState>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="A143:F143"/>
+    <mergeCell ref="A159:F159"/>
+    <mergeCell ref="A176:F176"/>
     <mergeCell ref="D67:E67"/>
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 3.17 bis,con pendientes
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07911BB1-2CBD-4FA7-A934-6C283C4FEEA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6526F0F4-36F9-41E6-BD47-1833493B326D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -468,13 +468,13 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
@@ -4549,6 +4549,1050 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DAB3-4313-9679-421D42FCAFA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Oferta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de un bien.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cantidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$71:$B$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9999999999944578E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$71:$A$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.3330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C15B-4FFF-BA11-4FEBCDBC3CDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Oferta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de un bien.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cantidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$87:$B$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$87:$A$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CDE0-4CF3-8C7E-40E7CEEC8A0F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9550,6 +10594,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -13693,6 +14817,1108 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -19267,6 +21493,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Gráfico 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{379B0585-81F1-4961-95FE-00DFE8BCFB2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Gráfico 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{185043AF-C90B-4736-9C6E-3D2632713EBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -19609,11 +21911,11 @@
       <c r="A3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="44">
         <f>F3</f>
         <v>3.0909979987868486E-2</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="43">
         <f>1/7</f>
         <v>0.14285714285714285</v>
       </c>
@@ -19621,11 +21923,11 @@
         <f>D2/E2</f>
         <v>1.2375</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="42">
         <f>D3^C3</f>
         <v>1.0309099799878685</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <f>E3-1</f>
         <v>3.0909979987868486E-2</v>
       </c>
@@ -19634,11 +21936,11 @@
       <c r="A4" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="44">
         <f>F4</f>
         <v>-2.9983199879617395E-2</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="43">
         <f>1/7</f>
         <v>0.14285714285714285</v>
       </c>
@@ -19646,29 +21948,29 @@
         <f>E2/D2</f>
         <v>0.80808080808080807</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="42">
         <f>D4^C4</f>
         <v>0.97001680012038261</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F4" s="42">
         <f>E4-1</f>
         <v>-2.9983199879617395E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="C5" s="44"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="C6" s="44"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="C7" s="44"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
@@ -19694,11 +21996,11 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <f>B9*(1+$F$3)</f>
+        <f t="shared" ref="B10:B16" si="0">B9*(1+$F$3)</f>
         <v>247.41839519708844</v>
       </c>
       <c r="D10">
-        <f>D9*(1+$F$4)</f>
+        <f t="shared" ref="D10:D16" si="1">D9*(1+$F$4)</f>
         <v>288.09498963575362</v>
       </c>
     </row>
@@ -19707,11 +22009,11 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <f>B10*(1+$F$3)</f>
+        <f t="shared" si="0"/>
         <v>255.066092841261</v>
       </c>
       <c r="D11">
-        <f>D10*(1+$F$4)</f>
+        <f t="shared" si="1"/>
         <v>279.4569799771885</v>
       </c>
     </row>
@@ -19720,11 +22022,11 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <f>B11*(1+$F$3)</f>
+        <f t="shared" si="0"/>
         <v>262.9501806665682</v>
       </c>
       <c r="D12">
-        <f>D11*(1+$F$4)</f>
+        <f t="shared" si="1"/>
         <v>271.0779654887782</v>
       </c>
     </row>
@@ -19733,11 +22035,11 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <f>B12*(1+$F$3)</f>
+        <f t="shared" si="0"/>
         <v>271.0779654887782</v>
       </c>
       <c r="D13">
-        <f>D12*(1+$F$4)</f>
+        <f t="shared" si="1"/>
         <v>262.95018066656814</v>
       </c>
     </row>
@@ -19746,11 +22048,11 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <f>B13*(1+$F$3)</f>
+        <f t="shared" si="0"/>
         <v>279.45697997718844</v>
       </c>
       <c r="D14">
-        <f>D13*(1+$F$4)</f>
+        <f t="shared" si="1"/>
         <v>255.06609284126094</v>
       </c>
     </row>
@@ -19759,11 +22061,11 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <f>B14*(1+$F$3)</f>
+        <f t="shared" si="0"/>
         <v>288.09498963575351</v>
       </c>
       <c r="D15">
-        <f>D14*(1+$F$4)</f>
+        <f t="shared" si="1"/>
         <v>247.41839519708836</v>
       </c>
     </row>
@@ -19772,11 +22074,11 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <f>B15*(1+$F$3)</f>
+        <f t="shared" si="0"/>
         <v>296.99999999999983</v>
       </c>
       <c r="D16">
-        <f>D15*(1+$F$4)</f>
+        <f t="shared" si="1"/>
         <v>239.99999999999989</v>
       </c>
     </row>
@@ -20859,10 +23161,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="42">
+      <c r="A1" s="46">
         <v>3.1</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
@@ -20921,10 +23223,10 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="42">
+      <c r="A17" s="46">
         <v>3.2</v>
       </c>
-      <c r="B17" s="42"/>
+      <c r="B17" s="46"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
@@ -20975,10 +23277,10 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="42">
+      <c r="A34" s="46">
         <v>3.3</v>
       </c>
-      <c r="B34" s="42"/>
+      <c r="B34" s="46"/>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
@@ -21037,10 +23339,10 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="42">
+      <c r="A51" s="46">
         <v>3.4</v>
       </c>
-      <c r="B51" s="42"/>
+      <c r="B51" s="46"/>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
@@ -21091,14 +23393,14 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="42">
+      <c r="A67" s="46">
         <v>3.5</v>
       </c>
-      <c r="B67" s="42"/>
-      <c r="D67" s="42">
+      <c r="B67" s="46"/>
+      <c r="D67" s="46">
         <v>3.5</v>
       </c>
-      <c r="E67" s="42"/>
+      <c r="E67" s="46"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
@@ -21354,14 +23656,14 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="42">
+      <c r="A92" s="46">
         <v>3.6</v>
       </c>
-      <c r="B92" s="42"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="42"/>
-      <c r="E92" s="42"/>
-      <c r="F92" s="42"/>
+      <c r="B92" s="46"/>
+      <c r="C92" s="46"/>
+      <c r="D92" s="46"/>
+      <c r="E92" s="46"/>
+      <c r="F92" s="46"/>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
@@ -21504,14 +23806,14 @@
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="42">
+      <c r="A110" s="46">
         <v>3.7</v>
       </c>
-      <c r="B110" s="42"/>
-      <c r="C110" s="42"/>
-      <c r="D110" s="42"/>
-      <c r="E110" s="42"/>
-      <c r="F110" s="42"/>
+      <c r="B110" s="46"/>
+      <c r="C110" s="46"/>
+      <c r="D110" s="46"/>
+      <c r="E110" s="46"/>
+      <c r="F110" s="46"/>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
@@ -21654,14 +23956,14 @@
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="42">
+      <c r="A127" s="46">
         <v>3.8</v>
       </c>
-      <c r="B127" s="42"/>
-      <c r="C127" s="42"/>
-      <c r="D127" s="42"/>
-      <c r="E127" s="42"/>
-      <c r="F127" s="42"/>
+      <c r="B127" s="46"/>
+      <c r="C127" s="46"/>
+      <c r="D127" s="46"/>
+      <c r="E127" s="46"/>
+      <c r="F127" s="46"/>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
@@ -21799,14 +24101,14 @@
       </c>
     </row>
     <row r="143" spans="1:6">
-      <c r="A143" s="42" t="s">
+      <c r="A143" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="B143" s="42"/>
-      <c r="C143" s="42"/>
-      <c r="D143" s="42"/>
-      <c r="E143" s="42"/>
-      <c r="F143" s="42"/>
+      <c r="B143" s="46"/>
+      <c r="C143" s="46"/>
+      <c r="D143" s="46"/>
+      <c r="E143" s="46"/>
+      <c r="F143" s="46"/>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
@@ -21944,14 +24246,14 @@
       </c>
     </row>
     <row r="159" spans="1:6">
-      <c r="A159" s="42" t="s">
+      <c r="A159" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="B159" s="42"/>
-      <c r="C159" s="42"/>
-      <c r="D159" s="42"/>
-      <c r="E159" s="42"/>
-      <c r="F159" s="42"/>
+      <c r="B159" s="46"/>
+      <c r="C159" s="46"/>
+      <c r="D159" s="46"/>
+      <c r="E159" s="46"/>
+      <c r="F159" s="46"/>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
@@ -22094,14 +24396,14 @@
       </c>
     </row>
     <row r="176" spans="1:6">
-      <c r="A176" s="42" t="s">
+      <c r="A176" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B176" s="42"/>
-      <c r="C176" s="42"/>
-      <c r="D176" s="42"/>
-      <c r="E176" s="42"/>
-      <c r="F176" s="42"/>
+      <c r="B176" s="46"/>
+      <c r="C176" s="46"/>
+      <c r="D176" s="46"/>
+      <c r="E176" s="46"/>
+      <c r="F176" s="46"/>
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
@@ -22243,11 +24545,6 @@
     <sortCondition ref="D69:D77"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A159:F159"/>
     <mergeCell ref="A176:F176"/>
@@ -22255,6 +24552,11 @@
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22265,19 +24567,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3DCD6C-8C16-46BB-BE84-B4869C965D7A}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="42">
+      <c r="A1" s="46">
         <v>3.12</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="46"/>
       <c r="C1">
         <v>100</v>
       </c>
@@ -22297,7 +24599,7 @@
       <c r="A3">
         <v>15</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <f>$C$1-A3*$C$2</f>
         <v>85</v>
       </c>
@@ -22348,10 +24650,10 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="42">
+      <c r="A19" s="46">
         <v>3.13</v>
       </c>
-      <c r="B19" s="42"/>
+      <c r="B19" s="46"/>
       <c r="C19">
         <v>40</v>
       </c>
@@ -22422,10 +24724,10 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="42">
+      <c r="A35" s="46">
         <v>3.14</v>
       </c>
-      <c r="B35" s="42"/>
+      <c r="B35" s="46"/>
       <c r="C35">
         <v>500</v>
       </c>
@@ -22496,10 +24798,10 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="42">
+      <c r="A51" s="46">
         <v>3.15</v>
       </c>
-      <c r="B51" s="42"/>
+      <c r="B51" s="46"/>
       <c r="C51">
         <v>80</v>
       </c>
@@ -22569,12 +24871,162 @@
         <v>0</v>
       </c>
     </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="46">
+        <v>3.16</v>
+      </c>
+      <c r="B69" s="46"/>
+      <c r="C69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>-5</v>
+      </c>
+      <c r="B71">
+        <f>$C$69+$C$70*A71</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>-3.3330000000000002</v>
+      </c>
+      <c r="B72">
+        <f>$C$69+$C$70*A72</f>
+        <v>9.9999999999944578E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>-2</v>
+      </c>
+      <c r="B73">
+        <f>$C$69+$C$70*A73</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>0</v>
+      </c>
+      <c r="B74">
+        <f>$C$69+$C$70*A74</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>5</v>
+      </c>
+      <c r="B75">
+        <f>$C$69+$C$70*A75</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>7</v>
+      </c>
+      <c r="B76">
+        <f>$C$69+$C$70*A76</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="46">
+        <v>3.17</v>
+      </c>
+      <c r="B85" s="46"/>
+      <c r="C85">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>-3</v>
+      </c>
+      <c r="B87">
+        <f>$C$85+$C$86*A87</f>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>-2</v>
+      </c>
+      <c r="B88">
+        <f t="shared" ref="B88:B92" si="4">$C$85+$C$86*A88</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>0</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="4"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>2.5</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>5</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>7</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A85:B85"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A69:B69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 3.18, pendientes de revision de 3.16-3.18
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6526F0F4-36F9-41E6-BD47-1833493B326D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44432BE-AFC3-4158-831E-33F59AA1EFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="72">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Q=10+3P</t>
+  </si>
+  <si>
+    <t>Q=-10+3P</t>
   </si>
 </sst>
 </file>
@@ -5880,6 +5886,644 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Oferta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de un bien (2 ecuaciones).</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$B$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q=-10+3P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$105:$B$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-19.999000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.9999999999944578E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$105:$A$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-3.3330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3330000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3C24-43CF-825F-5E08015013B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$C$104</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q=10+3P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$C$105:$C$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9.9999999999944578E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.999000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$105:$A$108</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-3.3330000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3330000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3C24-43CF-825F-5E08015013B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -10674,6 +11318,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -15919,6 +16603,557 @@
 </file>
 
 <file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -21569,6 +22804,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF96128-7A58-498B-B26E-C61B4B6DAD57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -24545,6 +25818,11 @@
     <sortCondition ref="D69:D77"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A159:F159"/>
     <mergeCell ref="A176:F176"/>
@@ -24552,11 +25830,6 @@
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24567,10 +25840,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3DCD6C-8C16-46BB-BE84-B4869C965D7A}">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:B92"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="K105" sqref="K105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -24896,7 +26169,7 @@
         <v>-5</v>
       </c>
       <c r="B71">
-        <f>$C$69+$C$70*A71</f>
+        <f t="shared" ref="B71:B76" si="4">$C$69+$C$70*A71</f>
         <v>-5</v>
       </c>
     </row>
@@ -24905,7 +26178,7 @@
         <v>-3.3330000000000002</v>
       </c>
       <c r="B72">
-        <f>$C$69+$C$70*A72</f>
+        <f t="shared" si="4"/>
         <v>9.9999999999944578E-4</v>
       </c>
     </row>
@@ -24914,7 +26187,7 @@
         <v>-2</v>
       </c>
       <c r="B73">
-        <f>$C$69+$C$70*A73</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -24923,7 +26196,7 @@
         <v>0</v>
       </c>
       <c r="B74">
-        <f>$C$69+$C$70*A74</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
     </row>
@@ -24932,7 +26205,7 @@
         <v>5</v>
       </c>
       <c r="B75">
-        <f>$C$69+$C$70*A75</f>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
     </row>
@@ -24941,7 +26214,7 @@
         <v>7</v>
       </c>
       <c r="B76">
-        <f>$C$69+$C$70*A76</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
     </row>
@@ -24979,7 +26252,7 @@
         <v>-2</v>
       </c>
       <c r="B88">
-        <f t="shared" ref="B88:B92" si="4">$C$85+$C$86*A88</f>
+        <f t="shared" ref="B88:B92" si="5">$C$85+$C$86*A88</f>
         <v>-9</v>
       </c>
     </row>
@@ -24988,7 +26261,7 @@
         <v>0</v>
       </c>
       <c r="B89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-5</v>
       </c>
     </row>
@@ -24997,7 +26270,7 @@
         <v>2.5</v>
       </c>
       <c r="B90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -25006,7 +26279,7 @@
         <v>5</v>
       </c>
       <c r="B91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -25015,12 +26288,80 @@
         <v>7</v>
       </c>
       <c r="B92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="46">
+        <v>3.18</v>
+      </c>
+      <c r="B102" s="46"/>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103">
+        <v>-10</v>
+      </c>
+      <c r="B103">
+        <v>3</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>26</v>
+      </c>
+      <c r="B104" t="s">
+        <v>71</v>
+      </c>
+      <c r="C104" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
+        <v>-3.3330000000000002</v>
+      </c>
+      <c r="B105">
+        <f>$A$103+$B$103*A105</f>
+        <v>-19.999000000000002</v>
+      </c>
+      <c r="C105">
+        <f>$C$103+$B$103*A105</f>
+        <v>9.9999999999944578E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>0</v>
+      </c>
+      <c r="B107">
+        <f>$A$103+$B$103*A107</f>
+        <v>-10</v>
+      </c>
+      <c r="C107">
+        <f>$C$103+$B$103*A107</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>3.3330000000000002</v>
+      </c>
+      <c r="B108">
+        <f>$A$103+$B$103*A108</f>
+        <v>-9.9999999999944578E-4</v>
+      </c>
+      <c r="C108">
+        <f>$C$103+$B$103*A108</f>
+        <v>19.999000000000002</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A102:B102"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A19:B19"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 3.20, siguen los pendientes
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44432BE-AFC3-4158-831E-33F59AA1EFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7721475-0317-45A9-A3C1-99FF5892637B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="76">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -249,6 +249,18 @@
   </si>
   <si>
     <t>Q=-10+3P</t>
+  </si>
+  <si>
+    <t>Q=-5+1/2P</t>
+  </si>
+  <si>
+    <t>Q=5+1/2P</t>
+  </si>
+  <si>
+    <t>Q=300-P</t>
+  </si>
+  <si>
+    <t>Q=300-1/2P</t>
   </si>
 </sst>
 </file>
@@ -7144,6 +7156,1318 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Oferta</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de un bien (2 ecuaciones).</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$B$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q=-5+1/2P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$119:$B$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$119:$A$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5CE8-4C47-83A1-FE1A65BD4C46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$C$118</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q=5+1/2P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$C$119:$C$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$119:$A$122</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5CE8-4C47-83A1-FE1A65BD4C46}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Demanda</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de un bien (2 ecuaciones).</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$B$135</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q=300-P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$136:$B$140</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$136:$A$140</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-41C9-47AC-BB31-0364EFC62823}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$C$135</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q=300-1/2P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$C$136:$C$140</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$136:$A$140</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-41C9-47AC-BB31-0364EFC62823}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Precio</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -11398,6 +12722,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors21.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17705,6 +19109,1108 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style21.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22842,6 +25348,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Gráfico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBBD57B9-EC4D-4E4F-9CD5-4F171908F3E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Gráfico 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4080EE8-C4F2-4844-873B-07959FBCB33A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -25818,11 +28400,6 @@
     <sortCondition ref="D69:D77"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A159:F159"/>
     <mergeCell ref="A176:F176"/>
@@ -25830,6 +28407,11 @@
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25840,10 +28422,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3DCD6C-8C16-46BB-BE84-B4869C965D7A}">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="K105" sqref="K105"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -26359,8 +28941,185 @@
         <v>19.999000000000002</v>
       </c>
     </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="46">
+        <v>3.19</v>
+      </c>
+      <c r="B116" s="46"/>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117">
+        <v>-5</v>
+      </c>
+      <c r="B117">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="C117">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" t="s">
+        <v>72</v>
+      </c>
+      <c r="C118" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119">
+        <v>-18</v>
+      </c>
+      <c r="B119">
+        <f>$A$117+$B$117*A119</f>
+        <v>-14</v>
+      </c>
+      <c r="C119">
+        <f>$C$117+$B$117*A119</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120">
+        <v>-10</v>
+      </c>
+      <c r="B120">
+        <f t="shared" ref="B120:B122" si="6">$A$117+$B$117*A120</f>
+        <v>-10</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ref="C120:C122" si="7">$C$117+$B$117*A120</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121">
+        <v>10</v>
+      </c>
+      <c r="B121">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122">
+        <v>18</v>
+      </c>
+      <c r="B122">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="46">
+        <v>3.2</v>
+      </c>
+      <c r="B133" s="46"/>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134">
+        <v>300</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>26</v>
+      </c>
+      <c r="B135" t="s">
+        <v>74</v>
+      </c>
+      <c r="C135" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136">
+        <v>600</v>
+      </c>
+      <c r="B136">
+        <f>$A$134-$B$134*A136</f>
+        <v>-300</v>
+      </c>
+      <c r="C136">
+        <f>$A$134-$C$134*A136</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137">
+        <v>300</v>
+      </c>
+      <c r="B137">
+        <f t="shared" ref="B137:B140" si="8">$A$134-$B$134*A137</f>
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <f t="shared" ref="C137:C140" si="9">$A$134-$C$134*A137</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138">
+        <v>150</v>
+      </c>
+      <c r="B138">
+        <f t="shared" si="8"/>
+        <v>150</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="9"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139">
+        <v>70</v>
+      </c>
+      <c r="B139">
+        <f t="shared" si="8"/>
+        <v>230</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="9"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140">
+        <v>0</v>
+      </c>
+      <c r="B140">
+        <f t="shared" si="8"/>
+        <v>300</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A133:B133"/>
     <mergeCell ref="A102:B102"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 3.31
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7721475-0317-45A9-A3C1-99FF5892637B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6681F176-910D-4DC6-A652-663F70519C54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="86">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -261,6 +261,36 @@
   </si>
   <si>
     <t>Q=300-1/2P</t>
+  </si>
+  <si>
+    <t>3.20</t>
+  </si>
+  <si>
+    <t>Ingreso (Y)</t>
+  </si>
+  <si>
+    <t>Consumo (C)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>C'</t>
+  </si>
+  <si>
+    <t>C autónomo</t>
+  </si>
+  <si>
+    <t>pMC</t>
+  </si>
+  <si>
+    <t>C=Co+4/5Y</t>
+  </si>
+  <si>
+    <t>C=Co+0.75Y</t>
   </si>
 </sst>
 </file>
@@ -8342,6 +8372,1851 @@
                 <a:r>
                   <a:rPr lang="es-MX" baseline="0"/>
                   <a:t> ($)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Función</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de consumo</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20115236857064889"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.74978838003361037"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$A$151</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Consumo (C)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$152:$B$156</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$152:$A$156</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-12AF-49D5-8D05-6ADD8EB72551}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Ingreso (Y) </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Consumo (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Función de consumo (2 ecuaciones).</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$A$167</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C'</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$168:$B$171</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$168:$A$171</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2B9E-4D32-9108-388514094B79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$C$167</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$D$168:$D$171</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$C$168:$C$171</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2B9E-4D32-9108-388514094B79}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Ingreso (Y) </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Consumo (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Función de consumo (2 ecuaciones).</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$A$187</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=Co+0.75Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$188:$B$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$188:$A$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>184.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>551</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1649</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4940</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF04-4787-AA89-AA8FDF1987D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$C$187</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=Co+4/5Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$D$188:$D$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>732</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2196</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6584</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$C$188:$C$193</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>196.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>587.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1758.8000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5269.2000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FF04-4787-AA89-AA8FDF1987D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Ingreso (Y) </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Consumo (C)</a:t>
                 </a:r>
                 <a:endParaRPr lang="es-MX"/>
               </a:p>
@@ -12802,6 +14677,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors22.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -20211,6 +22206,1659 @@
 </file>
 
 <file path=xl/charts/style21.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style22.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style24.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -25424,6 +29072,120 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Gráfico 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20BDE75F-2E1C-4157-B3B1-F2E73FF35748}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Gráfico 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53EAA1E3-0725-4687-9665-865259B3E41F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Gráfico 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{003CC1E4-8D1C-4811-81CA-C763EB3A3D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -28422,10 +32184,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3DCD6C-8C16-46BB-BE84-B4869C965D7A}">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -29023,8 +32785,8 @@
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="46">
-        <v>3.2</v>
+      <c r="A133" s="46" t="s">
+        <v>76</v>
       </c>
       <c r="B133" s="46"/>
     </row>
@@ -29116,17 +32878,295 @@
         <v>300</v>
       </c>
     </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="46">
+        <v>3.27</v>
+      </c>
+      <c r="B150" s="46"/>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>78</v>
+      </c>
+      <c r="B151" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152">
+        <v>0</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153">
+        <v>3</v>
+      </c>
+      <c r="B153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154">
+        <v>5</v>
+      </c>
+      <c r="B154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155">
+        <v>10</v>
+      </c>
+      <c r="B155">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156">
+        <v>18</v>
+      </c>
+      <c r="B156">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="46">
+        <v>3.28</v>
+      </c>
+      <c r="B166" s="46"/>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>81</v>
+      </c>
+      <c r="B167" t="s">
+        <v>80</v>
+      </c>
+      <c r="C167" t="s">
+        <v>79</v>
+      </c>
+      <c r="D167" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168">
+        <v>60</v>
+      </c>
+      <c r="B168">
+        <v>60</v>
+      </c>
+      <c r="C168">
+        <v>54</v>
+      </c>
+      <c r="D168">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169">
+        <v>80</v>
+      </c>
+      <c r="B169">
+        <v>80</v>
+      </c>
+      <c r="C169">
+        <v>90</v>
+      </c>
+      <c r="D169">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170">
+        <v>90</v>
+      </c>
+      <c r="B170">
+        <v>90</v>
+      </c>
+      <c r="C170">
+        <v>108</v>
+      </c>
+      <c r="D170">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171">
+        <v>160</v>
+      </c>
+      <c r="B171">
+        <v>160</v>
+      </c>
+      <c r="C171">
+        <v>144</v>
+      </c>
+      <c r="D171">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" s="46">
+        <v>3.31</v>
+      </c>
+      <c r="B184" s="46"/>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="s">
+        <v>82</v>
+      </c>
+      <c r="B185" t="s">
+        <v>83</v>
+      </c>
+      <c r="C185" t="s">
+        <v>82</v>
+      </c>
+      <c r="D185" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186">
+        <v>2</v>
+      </c>
+      <c r="B186">
+        <v>0.75</v>
+      </c>
+      <c r="C186">
+        <v>2</v>
+      </c>
+      <c r="D186">
+        <f>4/5</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="s">
+        <v>85</v>
+      </c>
+      <c r="B187" t="s">
+        <v>77</v>
+      </c>
+      <c r="C187" t="s">
+        <v>84</v>
+      </c>
+      <c r="D187" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188">
+        <f>$A$186+$B$186*B188</f>
+        <v>2.75</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188">
+        <f>$C$186+$D$186*D188</f>
+        <v>2.8</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189">
+        <f>$A$186+$B$186*B189</f>
+        <v>22.25</v>
+      </c>
+      <c r="B189">
+        <v>27</v>
+      </c>
+      <c r="C189">
+        <f>$C$186+$D$186*D189</f>
+        <v>23.6</v>
+      </c>
+      <c r="D189">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190">
+        <f t="shared" ref="A190:A193" si="10">$A$186+$B$186*B190</f>
+        <v>184.25</v>
+      </c>
+      <c r="B190">
+        <v>243</v>
+      </c>
+      <c r="C190">
+        <f t="shared" ref="C190:C193" si="11">$C$186+$D$186*D190</f>
+        <v>196.4</v>
+      </c>
+      <c r="D190">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191">
+        <f t="shared" si="10"/>
+        <v>551</v>
+      </c>
+      <c r="B191">
+        <v>732</v>
+      </c>
+      <c r="C191">
+        <f t="shared" si="11"/>
+        <v>587.6</v>
+      </c>
+      <c r="D191">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192">
+        <f t="shared" si="10"/>
+        <v>1649</v>
+      </c>
+      <c r="B192">
+        <v>2196</v>
+      </c>
+      <c r="C192">
+        <f t="shared" si="11"/>
+        <v>1758.8000000000002</v>
+      </c>
+      <c r="D192">
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193">
+        <f t="shared" si="10"/>
+        <v>4940</v>
+      </c>
+      <c r="B193">
+        <v>6584</v>
+      </c>
+      <c r="C193">
+        <f t="shared" si="11"/>
+        <v>5269.2000000000007</v>
+      </c>
+      <c r="D193">
+        <v>6584</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A102:B102"/>
+  <mergeCells count="12">
+    <mergeCell ref="A184:B184"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A102:B102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 3.37
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11739D6C-2BF4-4190-B78B-39AA8A483535}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4468600C-EA1A-484E-95E6-D552E3A912A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="96">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>C=1000+0.6(Y)</t>
+  </si>
+  <si>
+    <t>QD=145-0.5(P)</t>
+  </si>
+  <si>
+    <t>Precio (P)</t>
+  </si>
+  <si>
+    <t>QD=280-5(P)</t>
   </si>
 </sst>
 </file>
@@ -12794,6 +12803,543 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Ecuación de demanda.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$A$278</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QD=145-0.5(P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$279:$A$282</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$279:$B$282</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CF04-489B-85EF-5C4C64D899AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="95"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Cantidad (Q) </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Precio (P)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -13365,6 +13911,543 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Ecuación de demanda.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$A$296</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>QD=280-5(P)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$297:$A$300</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$297:$B$300</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5D7F-4B6D-808A-200D99222916}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Cantidad (Q) </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Precio (P)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -17371,7 +18454,87 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors30.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -29187,7 +30350,1109 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style30.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -34116,6 +36381,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>292</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="20" name="Gráfico 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B785F4E-76FE-434C-9965-7B9BAA174C12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>310</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="22" name="Gráfico 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD5F3811-A3EE-41A9-B786-D140D61ECD53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -37092,11 +39433,6 @@
     <sortCondition ref="D69:D77"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A159:F159"/>
     <mergeCell ref="A176:F176"/>
@@ -37104,6 +39440,11 @@
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37114,10 +39455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3DCD6C-8C16-46BB-BE84-B4869C965D7A}">
-  <dimension ref="A1:D263"/>
+  <dimension ref="A1:D300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="Q253" sqref="Q253"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="B303" sqref="B303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -38407,24 +40748,142 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="276" spans="1:2">
+      <c r="A276">
+        <v>145</v>
+      </c>
+      <c r="B276">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" s="46">
+        <v>3.36</v>
+      </c>
+      <c r="B277" s="46"/>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>93</v>
+      </c>
+      <c r="B278" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279">
+        <f>$A$276-$B$276*B279</f>
+        <v>145</v>
+      </c>
+      <c r="B279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280">
+        <f>$A$276-$B$276*B280</f>
+        <v>130</v>
+      </c>
+      <c r="B280">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281">
+        <f>$A$276-$B$276*B281</f>
+        <v>115</v>
+      </c>
+      <c r="B281">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282">
+        <f>$A$276-$B$276*B282</f>
+        <v>100</v>
+      </c>
+      <c r="B282">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2">
+      <c r="A294">
+        <v>280</v>
+      </c>
+      <c r="B294">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2">
+      <c r="A295" s="46">
+        <v>3.37</v>
+      </c>
+      <c r="B295" s="46"/>
+    </row>
+    <row r="296" spans="1:2">
+      <c r="A296" t="s">
+        <v>95</v>
+      </c>
+      <c r="B296" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2">
+      <c r="A297">
+        <f>$A$294-$B$294*B297</f>
+        <v>280</v>
+      </c>
+      <c r="B297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2">
+      <c r="A298">
+        <f t="shared" ref="A298:A301" si="8">$A$294-$B$294*B298</f>
+        <v>130</v>
+      </c>
+      <c r="B298">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2">
+      <c r="A299">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="B299">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2">
+      <c r="A300">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="B300">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A258:B258"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A221:B221"/>
-    <mergeCell ref="A240:B240"/>
-    <mergeCell ref="A184:B184"/>
+  <mergeCells count="18">
+    <mergeCell ref="A277:B277"/>
+    <mergeCell ref="A295:B295"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A150:B150"/>
     <mergeCell ref="A166:B166"/>
     <mergeCell ref="A116:B116"/>
     <mergeCell ref="A133:B133"/>
     <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A258:B258"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A221:B221"/>
+    <mergeCell ref="A240:B240"/>
+    <mergeCell ref="A184:B184"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 3.47
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FB8236-9888-4E6D-953D-A0C13F715AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E367DD02-7BC4-4878-82D1-D25B94F5EF47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="107">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>C=52.5+0.7(Y)</t>
+  </si>
+  <si>
+    <t>C=98+0.8(Y)</t>
+  </si>
+  <si>
+    <t>C=15+0.9(Y)</t>
   </si>
 </sst>
 </file>
@@ -16835,6 +16841,1068 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7BDB-4D23-B69D-CDC9E55073DC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Ingreso (Y) </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Consumo (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Función de consumo.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$A$410</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=98+0.8(Y)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$411:$B$413</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>740</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$411:$A$413</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>690</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3EDB-4B5E-8B43-715429E1D59A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Ingreso (Y) </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>Consumo (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Función de consumo.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11376159230096236"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.57540135608048981"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja3!$A$429</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C=15+0.9(Y)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja3!$B$430:$B$432</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>350</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja3!$A$430:$A$432</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>330</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D725-4726-8032-FA6AA31107A1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21477,6 +22545,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors36.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors37.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -37111,6 +38259,1108 @@
 </file>
 
 <file path=xl/charts/style35.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style36.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style37.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -42305,6 +44555,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>406</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>423</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="27" name="Gráfico 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9D6C49-FF9A-44C3-BB9A-39D3A8D6C6A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>425</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>442</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="28" name="Gráfico 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D39E3295-AA6D-44D0-AA7C-1A23BFE1E1CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -45281,11 +47607,6 @@
     <sortCondition ref="D69:D77"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A159:F159"/>
     <mergeCell ref="A176:F176"/>
@@ -45293,6 +47614,11 @@
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A127:F127"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45303,10 +47629,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3DCD6C-8C16-46BB-BE84-B4869C965D7A}">
-  <dimension ref="A1:D408"/>
+  <dimension ref="A1:D446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" workbookViewId="0">
-      <selection activeCell="A408" sqref="A408"/>
+    <sheetView tabSelected="1" topLeftCell="A439" workbookViewId="0">
+      <selection activeCell="A446" sqref="A446:B446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -47025,7 +49351,7 @@
     </row>
     <row r="406" spans="1:3">
       <c r="A406">
-        <v>52.5</v>
+        <v>98</v>
       </c>
     </row>
     <row r="407" spans="1:3">
@@ -47045,8 +49371,141 @@
         <v>102</v>
       </c>
     </row>
+    <row r="409" spans="1:3">
+      <c r="A409">
+        <v>540</v>
+      </c>
+      <c r="B409">
+        <v>530</v>
+      </c>
+      <c r="C409">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3">
+      <c r="A410" t="s">
+        <v>105</v>
+      </c>
+      <c r="B410" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3">
+      <c r="A411">
+        <f>$A$406+$C$409*B411</f>
+        <v>370</v>
+      </c>
+      <c r="B411">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3">
+      <c r="A412">
+        <f t="shared" ref="A412:A413" si="14">$A$406+$C$409*B412</f>
+        <v>530</v>
+      </c>
+      <c r="B412">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3">
+      <c r="A413">
+        <f t="shared" si="14"/>
+        <v>690</v>
+      </c>
+      <c r="B413">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3">
+      <c r="A425">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3">
+      <c r="A426" s="46">
+        <v>3.47</v>
+      </c>
+      <c r="B426" s="46"/>
+    </row>
+    <row r="427" spans="1:3">
+      <c r="A427" t="s">
+        <v>100</v>
+      </c>
+      <c r="B427" t="s">
+        <v>101</v>
+      </c>
+      <c r="C427" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3">
+      <c r="A428">
+        <v>350</v>
+      </c>
+      <c r="B428">
+        <v>330</v>
+      </c>
+      <c r="C428">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3">
+      <c r="A429" t="s">
+        <v>106</v>
+      </c>
+      <c r="B429" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3">
+      <c r="A430">
+        <f>$A$425+$C$428*B430</f>
+        <v>60</v>
+      </c>
+      <c r="B430">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3">
+      <c r="A431">
+        <f t="shared" ref="A431:A432" si="15">$A$425+$C$428*B431</f>
+        <v>240</v>
+      </c>
+      <c r="B431">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3">
+      <c r="A432">
+        <f t="shared" si="15"/>
+        <v>330</v>
+      </c>
+      <c r="B432">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2">
+      <c r="A446" s="46">
+        <v>3.48</v>
+      </c>
+      <c r="B446" s="46"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
+    <mergeCell ref="A426:B426"/>
+    <mergeCell ref="A446:B446"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A369:B369"/>
     <mergeCell ref="A389:B389"/>
     <mergeCell ref="A407:B407"/>
@@ -47057,17 +49516,6 @@
     <mergeCell ref="A351:B351"/>
     <mergeCell ref="A277:B277"/>
     <mergeCell ref="A295:B295"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A102:B102"/>
     <mergeCell ref="A258:B258"/>
     <mergeCell ref="A202:B202"/>
     <mergeCell ref="A221:B221"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 3.61. Fin del capitulo 3.
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E367DD02-7BC4-4878-82D1-D25B94F5EF47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1458B420-99B3-47F7-ACE7-EA9FCF1B9364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja2" sheetId="3" r:id="rId1"/>
     <sheet name="Ejercicio 2.83" sheetId="1" r:id="rId2"/>
     <sheet name="Ejercicios 3.1-3.11" sheetId="2" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="4" r:id="rId4"/>
+    <sheet name="Ejercicios 3.12-3.47" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2997,7 +2997,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$2</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3044,7 +3044,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$3:$B$8</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3071,7 +3071,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$3:$A$8</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3519,7 +3519,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$20</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3566,7 +3566,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$21:$B$26</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$21:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3593,7 +3593,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$21:$A$26</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$21:$A$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4041,7 +4041,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$K$27</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$K$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -4085,7 +4085,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$37:$B$42</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$37:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4112,7 +4112,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$37:$A$42</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$37:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4560,7 +4560,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$52</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4607,7 +4607,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$53:$B$58</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$53:$B$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -4634,7 +4634,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$53:$A$58</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$53:$A$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5082,7 +5082,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$52</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5129,7 +5129,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$71:$B$76</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$71:$B$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5156,7 +5156,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$71:$A$76</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$71:$A$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5604,7 +5604,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$52</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5651,7 +5651,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$87:$B$92</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$87:$B$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -5678,7 +5678,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$87:$A$92</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$87:$A$92</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -6126,7 +6126,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$104</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$104</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6175,7 +6175,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$105:$B$108</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$105:$B$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -6193,7 +6193,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$105:$A$108</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$105:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -6221,7 +6221,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$104</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$104</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6268,7 +6268,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$C$105:$C$108</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$105:$C$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -6286,7 +6286,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$105:$A$108</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$105:$A$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -7384,7 +7384,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$118</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$118</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7433,7 +7433,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$119:$B$122</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$119:$B$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -7454,7 +7454,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$119:$A$122</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$119:$A$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -7485,7 +7485,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$118</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$118</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7532,7 +7532,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$C$119:$C$122</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$119:$C$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -7553,7 +7553,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$119:$A$122</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$119:$A$122</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8034,7 +8034,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$135</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$135</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8083,7 +8083,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$136:$B$140</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$136:$B$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8107,7 +8107,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$136:$A$140</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$136:$A$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8141,7 +8141,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$135</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$135</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8188,7 +8188,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$C$136:$C$140</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$136:$C$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8212,7 +8212,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$136:$A$140</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$136:$A$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8696,7 +8696,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$151</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$151</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8745,7 +8745,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$152:$B$156</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$152:$B$156</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8769,7 +8769,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$152:$A$156</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$152:$A$156</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -9237,7 +9237,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$167</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$167</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9286,7 +9286,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$168:$B$171</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$168:$B$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9307,7 +9307,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$168:$A$171</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$168:$A$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9338,7 +9338,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$167</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$167</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9385,7 +9385,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$D$168:$D$171</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$D$168:$D$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9406,7 +9406,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$C$168:$C$171</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$168:$C$171</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9875,7 +9875,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$187</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$187</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9924,7 +9924,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$188:$B$193</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$188:$B$193</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -9951,7 +9951,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$188:$A$193</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$188:$A$193</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -9988,7 +9988,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$187</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$187</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10035,7 +10035,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$D$188:$D$193</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$D$188:$D$193</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10062,7 +10062,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$C$188:$C$193</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$188:$C$193</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -10537,7 +10537,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$205</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$205</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10586,7 +10586,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$206:$B$209</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$206:$B$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -10607,7 +10607,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$206:$A$209</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$206:$A$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -10638,7 +10638,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$205</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$205</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10685,7 +10685,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$D$206:$D$209</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$D$206:$D$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -10706,7 +10706,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$C$206:$C$209</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$206:$C$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -11175,7 +11175,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$224</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$224</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11224,7 +11224,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$225:$B$226</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$225:$B$226</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -11239,7 +11239,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$225:$A$226</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$225:$A$226</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -11264,7 +11264,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$224</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$224</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11311,7 +11311,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$D$225:$D$226</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$D$225:$D$226</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -11326,7 +11326,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$C$225:$C$226</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$225:$C$226</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -11789,7 +11789,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$243</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$243</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11838,7 +11838,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$244:$B$245</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$244:$B$245</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -11853,7 +11853,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$244:$A$245</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$244:$A$245</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -11878,7 +11878,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$C$243</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$243</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11925,7 +11925,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$D$244:$D$245</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$D$244:$D$245</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -11940,7 +11940,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$C$244:$C$245</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$C$244:$C$245</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -12405,7 +12405,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$261</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$261</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12454,7 +12454,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$262:$B$263</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$262:$B$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -12469,7 +12469,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$262:$A$263</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$262:$A$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -12930,7 +12930,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$278</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$278</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12979,7 +12979,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$A$279:$A$282</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$279:$A$282</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -13000,7 +13000,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$B$279:$B$282</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$279:$B$282</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -14075,7 +14075,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$296</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$296</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -14124,7 +14124,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$A$297:$A$300</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$297:$A$300</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -14145,7 +14145,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$B$297:$B$300</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$297:$B$300</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -14612,7 +14612,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$313</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$313</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -14661,7 +14661,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$A$314:$A$317</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$314:$A$317</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -14682,7 +14682,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$B$314:$B$317</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$314:$B$317</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -15149,7 +15149,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$333</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$333</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -15198,7 +15198,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$A$334:$A$337</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$334:$A$337</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -15219,7 +15219,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$B$334:$B$337</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$334:$B$337</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -15686,7 +15686,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$352</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$352</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -15735,7 +15735,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$A$353:$A$356</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$353:$A$356</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -15756,7 +15756,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$B$353:$B$356</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$353:$B$356</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -16223,7 +16223,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$372</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$372</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -16272,7 +16272,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$373:$B$375</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$373:$B$375</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -16290,7 +16290,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$373:$A$375</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$373:$A$375</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -16754,7 +16754,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$392</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$392</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -16803,7 +16803,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$393:$B$395</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$393:$B$395</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -16821,7 +16821,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$393:$A$395</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$393:$A$395</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -17285,7 +17285,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$410</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$410</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -17334,7 +17334,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$411:$B$413</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$411:$B$413</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -17352,7 +17352,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$411:$A$413</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$411:$A$413</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -17816,7 +17816,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$A$429</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$429</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -17865,7 +17865,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$B$430:$B$432</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$B$430:$B$432</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -17883,7 +17883,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$A$430:$A$432</c:f>
+              <c:f>'Ejercicios 3.12-3.47'!$A$430:$A$432</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -47607,6 +47607,11 @@
     <sortCondition ref="D69:D77"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A159:F159"/>
     <mergeCell ref="A176:F176"/>
@@ -47614,11 +47619,6 @@
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -47629,10 +47629,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3DCD6C-8C16-46BB-BE84-B4869C965D7A}">
-  <dimension ref="A1:D446"/>
+  <dimension ref="A1:D432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A439" workbookViewId="0">
-      <selection activeCell="A446" sqref="A446:B446"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -49485,27 +49485,25 @@
         <v>350</v>
       </c>
     </row>
-    <row r="446" spans="1:2">
-      <c r="A446" s="46">
-        <v>3.48</v>
-      </c>
-      <c r="B446" s="46"/>
-    </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="25">
+    <mergeCell ref="A277:B277"/>
+    <mergeCell ref="A295:B295"/>
+    <mergeCell ref="A258:B258"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A221:B221"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A426:B426"/>
-    <mergeCell ref="A446:B446"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A150:B150"/>
     <mergeCell ref="A166:B166"/>
     <mergeCell ref="A116:B116"/>
     <mergeCell ref="A133:B133"/>
     <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A369:B369"/>
     <mergeCell ref="A389:B389"/>
     <mergeCell ref="A407:B407"/>
@@ -49514,11 +49512,6 @@
     <mergeCell ref="A312:B312"/>
     <mergeCell ref="A332:B332"/>
     <mergeCell ref="A351:B351"/>
-    <mergeCell ref="A277:B277"/>
-    <mergeCell ref="A295:B295"/>
-    <mergeCell ref="A258:B258"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A221:B221"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion hasta el ejercicio 4.43
</commit_message>
<xml_diff>
--- a/ConsultaDeDatos.xlsx
+++ b/ConsultaDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANGEL\Documents\Fundamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C3F3BB-66FB-47CB-9655-6C46B650578E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCCCCD3-5C9C-4D15-AA85-D656ABED19C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{D981B6FC-7059-4534-899D-D6159089EF04}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="114">
   <si>
     <t>Deflactor implícito del PIB</t>
   </si>
@@ -24610,8 +24610,10 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -24632,20 +24634,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$A$136:$A$138</c:f>
@@ -24704,8 +24692,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -24726,20 +24717,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="dash"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$A$140:$A$142</c:f>
@@ -24798,8 +24775,11 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -24820,19 +24800,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Hoja1!$A$144:$A$146</c:f>
@@ -25153,28 +25120,1951 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="0"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="2"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Funciones</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout>
         <c:manualLayout>
+          <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20713167104111985"/>
-          <c:y val="0.92187445319335082"/>
-          <c:w val="0.64711832895888011"/>
-          <c:h val="7.8125546806649182E-2"/>
+          <c:x val="9.987270341207348E-2"/>
+          <c:y val="0.1413425925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
         </c:manualLayout>
       </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$150</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$151:$A$153</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$151:$B$153</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6A22-4F88-8097-0430B9C59873}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$155</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$155:$A$157</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$155:$B$157</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7777777777777776E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6A22-4F88-8097-0430B9C59873}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$159</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$159:$A$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$159:$B$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7037037037037035E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6296296296296294E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-6A22-4F88-8097-0430B9C59873}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>x </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Funciones</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.987270341207348E-2"/>
+          <c:y val="0.1413425925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$165</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$166:$A$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$166:$B$168</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.33333333333333331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65B4-4001-8D02-1AC47DBB3AD9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$170</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$170:$A$172</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$170:$B$172</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.6666666666666666E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-65B4-4001-8D02-1AC47DBB3AD9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>x </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Funciones</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.987270341207348E-2"/>
+          <c:y val="0.1413425925925926"/>
+          <c:w val="0.84734951881014875"/>
+          <c:h val="0.61706802274715655"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$181</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>a</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="dashDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$182:$A$184</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$182:$B$184</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1860-4A2F-A634-74CC9FA50282}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$186</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>b</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$186:$A$188</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$186:$B$189</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1860-4A2F-A634-74CC9FA50282}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$190</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="15875">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$A$190:$A$192</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$B$190:$B$192</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1860-4A2F-A634-74CC9FA50282}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689605439"/>
+        <c:axId val="634792095"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689605439"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="51000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX" baseline="0"/>
+                  <a:t>x </a:t>
+                </a:r>
+                <a:endParaRPr lang="es-MX"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="634792095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="634792095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>y</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-MX"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689605439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -29447,6 +31337,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors46.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors47.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors48.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -51102,6 +53112,1659 @@
 </file>
 
 <file path=xl/charts/style45.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style46.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style47.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style48.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -56130,6 +59793,120 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC8B379C-3A52-4251-931C-60BF608664A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Gráfico 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6C9F69-7EA6-4E37-9117-FC0DBA1224CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Gráfico 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C606FE4C-E828-4B31-BED0-5C0790B92A52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -59106,6 +62883,11 @@
     <sortCondition ref="D69:D77"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A67:B67"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A159:F159"/>
     <mergeCell ref="A176:F176"/>
@@ -59113,11 +62895,6 @@
     <mergeCell ref="A92:F92"/>
     <mergeCell ref="A110:F110"/>
     <mergeCell ref="A127:F127"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A67:B67"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -60986,6 +64763,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A295:B295"/>
+    <mergeCell ref="A258:B258"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="A221:B221"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A426:B426"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A150:B150"/>
@@ -61001,16 +64787,7 @@
     <mergeCell ref="A312:B312"/>
     <mergeCell ref="A332:B332"/>
     <mergeCell ref="A351:B351"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A69:B69"/>
     <mergeCell ref="A277:B277"/>
-    <mergeCell ref="A295:B295"/>
-    <mergeCell ref="A258:B258"/>
-    <mergeCell ref="A202:B202"/>
-    <mergeCell ref="A221:B221"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -61020,13 +64797,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B454205-E29C-43D7-AC57-F06E9D79FEA5}">
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="46">
@@ -62022,7 +65802,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:3">
       <c r="A145">
         <v>3</v>
       </c>
@@ -62031,7 +65811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:3">
       <c r="A146">
         <v>9</v>
       </c>
@@ -62040,8 +65820,293 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="46">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="B149" s="46"/>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>108</v>
+      </c>
+      <c r="B150" t="s">
+        <v>107</v>
+      </c>
+      <c r="C150" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <f>1/A151</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152">
+        <v>3</v>
+      </c>
+      <c r="B152">
+        <f t="shared" ref="B152:B153" si="30">1/A152</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153">
+        <v>6</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="30"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <f>1/A155^2</f>
+        <v>1</v>
+      </c>
+      <c r="C155" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156">
+        <v>3</v>
+      </c>
+      <c r="B156">
+        <f t="shared" ref="B156:B157" si="31">1/A156^2</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157">
+        <v>6</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="31"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159">
+        <v>1</v>
+      </c>
+      <c r="B159">
+        <f>1/A159^3</f>
+        <v>1</v>
+      </c>
+      <c r="C159" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160">
+        <v>3</v>
+      </c>
+      <c r="B160">
+        <f t="shared" ref="B160:B161" si="32">1/A160^3</f>
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161">
+        <v>6</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="32"/>
+        <v>4.6296296296296294E-3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="46">
+        <v>4.28</v>
+      </c>
+      <c r="B164" s="46"/>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>108</v>
+      </c>
+      <c r="B165" t="s">
+        <v>107</v>
+      </c>
+      <c r="C165" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166">
+        <v>2</v>
+      </c>
+      <c r="B166">
+        <f>1/(1-A166)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167">
+        <v>3</v>
+      </c>
+      <c r="B167">
+        <f t="shared" ref="B167:B168" si="33">1/(1-A167)</f>
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168">
+        <v>4</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="33"/>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170">
+        <v>2</v>
+      </c>
+      <c r="B170">
+        <f>1/(1-A170^2)</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="C170" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171">
+        <v>3</v>
+      </c>
+      <c r="B171">
+        <f t="shared" ref="B171:B172" si="34">1/(1-A171^2)</f>
+        <v>-0.125</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172">
+        <v>4</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="34"/>
+        <v>-6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="46">
+        <v>4.29</v>
+      </c>
+      <c r="B180" s="46"/>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
+        <v>108</v>
+      </c>
+      <c r="B181" t="s">
+        <v>107</v>
+      </c>
+      <c r="C181" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182">
+        <v>2</v>
+      </c>
+      <c r="B182">
+        <f>1/A182^2</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183">
+        <v>3</v>
+      </c>
+      <c r="B183">
+        <f t="shared" ref="B183:B184" si="35">1/A183^2</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184">
+        <v>4</v>
+      </c>
+      <c r="B184">
+        <f t="shared" si="35"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186">
+        <v>2</v>
+      </c>
+      <c r="B186">
+        <f>3/(A186^2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C186" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187">
+        <v>3</v>
+      </c>
+      <c r="B187">
+        <f t="shared" ref="B187:B188" si="36">3/(A187^2)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188">
+        <v>4</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="36"/>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190">
+        <v>2</v>
+      </c>
+      <c r="B190">
+        <f>6/(A190^2)</f>
+        <v>1.5</v>
+      </c>
+      <c r="C190" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191">
+        <v>3</v>
+      </c>
+      <c r="B191">
+        <f t="shared" ref="B191:B192" si="37">6/(A191^2)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192">
+        <v>4</v>
+      </c>
+      <c r="B192">
+        <f t="shared" si="37"/>
+        <v>0.375</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A180:B180"/>
     <mergeCell ref="A118:B118"/>
     <mergeCell ref="A134:B134"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>